<commit_message>
EDSF-55: Can now send results page emails to users of the website, so freaking cool!
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-Scenario-Data.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-Scenario-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6057D8-4D82-4385-B9B7-6ECBC1F050A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51C01B8-E0FD-41F8-BDB6-8CED515BEC87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="5610" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="2730" windowWidth="14670" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Scenarios!$B$2:$X$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Scenarios!$B$2:$Y$5</definedName>
     <definedName name="Assumptions_TargetEnd_Scenario2">'[1]Assumptions - Dropouts'!$F$4</definedName>
     <definedName name="Assumptions_TargetEnd_Scenario3">'[1]Assumptions - Dropouts'!$F$5</definedName>
     <definedName name="Assumptions_TargetEnd_Scenario4">'[1]Assumptions - Dropouts'!$F$6</definedName>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>Scenario</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>For-Profit College</t>
+  </si>
+  <si>
+    <t>Margin</t>
   </si>
 </sst>
 </file>
@@ -362,18 +365,16 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -391,19 +392,10 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -424,16 +416,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -782,44 +772,45 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B2:X9"/>
+  <dimension ref="B2:Y9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C8" sqref="C8"/>
       <selection pane="topRight" activeCell="C8" sqref="C8"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.7109375" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -829,306 +820,318 @@
         <v>48</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="P2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="R2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="S2" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="T2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="W2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="10">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
+        <v>0.25</v>
+      </c>
+      <c r="F3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="27">
+      <c r="G3" s="21">
         <v>0.25</v>
       </c>
-      <c r="G3" s="27">
+      <c r="H3" s="21">
         <v>0.5</v>
       </c>
-      <c r="H3" s="27">
+      <c r="I3" s="21">
         <v>0.25</v>
       </c>
-      <c r="I3" s="30">
+      <c r="J3" s="4">
         <v>36.871688739980776</v>
       </c>
-      <c r="J3" s="31">
+      <c r="K3" s="24">
         <v>18.077297612212142</v>
       </c>
-      <c r="K3" s="30">
+      <c r="L3" s="4">
         <v>3.9588553533675892</v>
       </c>
-      <c r="L3" s="32">
-        <f>100-SUM(I3:K3)</f>
+      <c r="M3" s="25">
+        <f>100-SUM(J3:L3)</f>
         <v>41.092158294439493</v>
       </c>
-      <c r="M3" s="9">
-        <f>100-L3-SUM(N3:O3)-E3</f>
+      <c r="N3" s="7">
+        <f>100-M3-SUM(O3:P3)-F3</f>
         <v>37.907841705560507</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>10</v>
       </c>
-      <c r="O3" s="33">
+      <c r="P3" s="26">
         <v>6</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>36</v>
       </c>
-      <c r="Q3" s="29">
+      <c r="R3" s="23">
         <v>0</v>
       </c>
-      <c r="R3" s="29">
-        <f>Q3 * (12 / S3)</f>
+      <c r="S3" s="23">
+        <f>R3 * (12 / T3)</f>
         <v>0</v>
       </c>
-      <c r="S3" s="29">
-        <v>1</v>
-      </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="23">
+        <v>1</v>
+      </c>
+      <c r="U3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="V3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V3" s="29">
-        <v>1</v>
-      </c>
-      <c r="W3" s="7">
+      <c r="W3" s="23">
+        <v>1</v>
+      </c>
+      <c r="X3" s="3">
         <v>0</v>
       </c>
-      <c r="X3" s="8">
+      <c r="Y3" s="6">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
         <f>B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
+        <v>0.25</v>
+      </c>
+      <c r="F4" s="2">
         <v>5</v>
       </c>
-      <c r="F4" s="27">
+      <c r="G4" s="21">
         <v>0.25</v>
       </c>
-      <c r="G4" s="27">
+      <c r="H4" s="21">
         <v>0.5</v>
       </c>
-      <c r="H4" s="27">
+      <c r="I4" s="21">
         <v>0.25</v>
       </c>
-      <c r="I4" s="30">
+      <c r="J4" s="4">
         <v>54.298366358291453</v>
       </c>
-      <c r="J4" s="31">
+      <c r="K4" s="24">
         <v>9.8466660264413051</v>
       </c>
-      <c r="K4" s="30">
+      <c r="L4" s="4">
         <v>1.7125985295518689</v>
       </c>
-      <c r="L4" s="32">
-        <f t="shared" ref="L4:L5" si="0">100-SUM(I4:K4)</f>
+      <c r="M4" s="25">
+        <f t="shared" ref="M4:M5" si="0">100-SUM(J4:L4)</f>
         <v>34.142369085715373</v>
       </c>
-      <c r="M4" s="9">
-        <f t="shared" ref="M4:M5" si="1">100-L4-SUM(N4:O4)-E4</f>
+      <c r="N4" s="7">
+        <f t="shared" ref="N4:N5" si="1">100-M4-SUM(O4:P4)-F4</f>
         <v>39.857630914284627</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>18</v>
       </c>
-      <c r="O4" s="33">
+      <c r="P4" s="26">
         <v>2.9999999999999956</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>24</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="R4" s="23">
         <v>0</v>
       </c>
-      <c r="R4" s="29">
-        <f t="shared" ref="R4:R5" si="2">Q4 * (12 / S4)</f>
+      <c r="S4" s="23">
+        <f t="shared" ref="S4:S5" si="2">R4 * (12 / T4)</f>
         <v>0</v>
       </c>
-      <c r="S4" s="29">
-        <v>1</v>
-      </c>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="23">
+        <v>1</v>
+      </c>
+      <c r="U4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="15" t="s">
+      <c r="V4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="29">
-        <v>1</v>
-      </c>
-      <c r="W4" s="7">
+      <c r="W4" s="23">
+        <v>1</v>
+      </c>
+      <c r="X4" s="3">
         <v>0</v>
       </c>
-      <c r="X4" s="8">
+      <c r="Y4" s="6">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="10">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
         <f t="shared" ref="B5" si="3">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="27">
+      <c r="G5" s="21">
         <v>0.25</v>
       </c>
-      <c r="G5" s="27">
+      <c r="H5" s="21">
         <v>0.5</v>
       </c>
-      <c r="H5" s="27">
+      <c r="I5" s="21">
         <v>0.25</v>
       </c>
-      <c r="I5" s="30">
+      <c r="J5" s="4">
         <v>14.5079231933478</v>
       </c>
-      <c r="J5" s="31">
+      <c r="K5" s="24">
         <v>4.4493882091212456</v>
       </c>
-      <c r="K5" s="30">
+      <c r="L5" s="4">
         <v>1.8745783110559984</v>
       </c>
-      <c r="L5" s="32">
+      <c r="M5" s="25">
         <f t="shared" si="0"/>
         <v>79.168110286474956</v>
       </c>
-      <c r="M5" s="9">
+      <c r="N5" s="7">
         <f t="shared" si="1"/>
         <v>5.8318897135250438</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>0</v>
       </c>
-      <c r="O5" s="33">
+      <c r="P5" s="26">
         <v>10</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>42</v>
       </c>
-      <c r="Q5" s="29">
+      <c r="R5" s="23">
         <v>0</v>
       </c>
-      <c r="R5" s="29">
+      <c r="S5" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S5" s="29">
-        <v>1</v>
-      </c>
-      <c r="T5" s="15" t="s">
+      <c r="T5" s="23">
+        <v>1</v>
+      </c>
+      <c r="U5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="15" t="s">
+      <c r="V5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="29">
-        <v>1</v>
-      </c>
-      <c r="W5" s="7">
+      <c r="W5" s="23">
+        <v>1</v>
+      </c>
+      <c r="X5" s="3">
         <v>0</v>
       </c>
-      <c r="X5" s="8">
+      <c r="Y5" s="6">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:X5" xr:uid="{41D0623F-35E4-467D-8335-5335D24492F3}"/>
+  <autoFilter ref="B2:Y5" xr:uid="{41D0623F-35E4-467D-8335-5335D24492F3}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U5" xr:uid="{3EE6BC6F-6AD2-4260-AAC6-BB0AE485DC9E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3:V5" xr:uid="{3EE6BC6F-6AD2-4260-AAC6-BB0AE485DC9E}">
       <formula1>InterestRateTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -1172,10 +1175,10 @@
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1186,10 +1189,10 @@
       <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="3">
         <v>100</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>12</v>
       </c>
     </row>
@@ -1197,10 +1200,10 @@
       <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="3">
         <v>25</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>12</v>
       </c>
     </row>
@@ -1208,10 +1211,10 @@
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="3">
         <v>25</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>12</v>
       </c>
     </row>
@@ -1219,10 +1222,10 @@
       <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="3">
         <v>20</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1230,10 +1233,10 @@
       <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="3">
         <v>150</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="8"/>
       <c r="E7" t="s">
         <v>38</v>
       </c>
@@ -1242,10 +1245,10 @@
       <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="3">
         <v>150</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="8"/>
       <c r="E8" t="s">
         <v>40</v>
       </c>
@@ -1254,10 +1257,10 @@
       <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="3">
         <v>300</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="8"/>
       <c r="E9" t="s">
         <v>39</v>
       </c>
@@ -1266,10 +1269,10 @@
       <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="3">
         <v>1000</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="8"/>
       <c r="E10" t="s">
         <v>41</v>
       </c>
@@ -1302,75 +1305,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="8">
         <v>0</v>
       </c>
       <c r="B5" s="3">
@@ -1387,7 +1390,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="8">
         <v>1</v>
       </c>
       <c r="B6" s="3">
@@ -1404,7 +1407,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="8">
         <v>2</v>
       </c>
       <c r="B7" s="3">
@@ -1421,7 +1424,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="8">
         <v>3</v>
       </c>
       <c r="B8" s="3">
@@ -1438,7 +1441,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="8">
         <v>4</v>
       </c>
       <c r="B9" s="3">
@@ -1455,7 +1458,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="8">
         <v>5</v>
       </c>
       <c r="B10" s="3">
@@ -1472,7 +1475,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="8">
         <v>6</v>
       </c>
       <c r="B11" s="3">
@@ -1489,7 +1492,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="8">
         <v>7</v>
       </c>
       <c r="B12" s="3">
@@ -1506,7 +1509,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+      <c r="A13" s="8">
         <v>8</v>
       </c>
       <c r="B13" s="3">
@@ -1523,7 +1526,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+      <c r="A14" s="8">
         <v>9</v>
       </c>
       <c r="B14" s="3">
@@ -1540,7 +1543,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="A15" s="8">
         <v>10</v>
       </c>
       <c r="B15" s="3">
@@ -1557,7 +1560,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+      <c r="A16" s="8">
         <v>11</v>
       </c>
       <c r="B16" s="3">
@@ -1574,7 +1577,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+      <c r="A17" s="8">
         <v>12</v>
       </c>
       <c r="B17" s="3">
@@ -1591,7 +1594,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="A18" s="8">
         <v>13</v>
       </c>
       <c r="B18" s="3">
@@ -1608,7 +1611,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+      <c r="A19" s="8">
         <v>14</v>
       </c>
       <c r="B19" s="3">
@@ -1625,7 +1628,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+      <c r="A20" s="8">
         <v>15</v>
       </c>
       <c r="B20" s="3">
@@ -1642,7 +1645,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="A21" s="8">
         <v>16</v>
       </c>
       <c r="B21" s="3">
@@ -1659,7 +1662,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+      <c r="A22" s="8">
         <v>17</v>
       </c>
       <c r="B22" s="3">
@@ -1676,7 +1679,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+      <c r="A23" s="8">
         <v>18</v>
       </c>
       <c r="B23" s="3">
@@ -1693,7 +1696,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+      <c r="A24" s="8">
         <v>19</v>
       </c>
       <c r="B24" s="3">
@@ -1710,7 +1713,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
+      <c r="A25" s="8">
         <v>20</v>
       </c>
       <c r="B25" s="3">
@@ -1727,7 +1730,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+      <c r="A26" s="8">
         <v>21</v>
       </c>
       <c r="B26" s="3">
@@ -1744,7 +1747,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+      <c r="A27" s="8">
         <v>22</v>
       </c>
       <c r="B27" s="3">
@@ -1761,7 +1764,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
+      <c r="A28" s="8">
         <v>23</v>
       </c>
       <c r="B28" s="3">
@@ -1778,7 +1781,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
+      <c r="A29" s="8">
         <v>24</v>
       </c>
       <c r="B29" s="3">
@@ -1795,7 +1798,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+      <c r="A30" s="8">
         <v>25</v>
       </c>
       <c r="B30" s="3">
@@ -1812,7 +1815,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
+      <c r="A31" s="8">
         <v>26</v>
       </c>
       <c r="B31" s="3">
@@ -1829,7 +1832,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+      <c r="A32" s="8">
         <v>27</v>
       </c>
       <c r="B32" s="3">
@@ -1846,7 +1849,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
+      <c r="A33" s="8">
         <v>28</v>
       </c>
       <c r="B33" s="3">
@@ -1863,7 +1866,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
+      <c r="A34" s="8">
         <v>29</v>
       </c>
       <c r="B34" s="3">
@@ -1880,7 +1883,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
+      <c r="A35" s="8">
         <v>30</v>
       </c>
       <c r="B35" s="3">
@@ -1897,7 +1900,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+      <c r="A36" s="8">
         <v>31</v>
       </c>
       <c r="B36" s="3">
@@ -1914,7 +1917,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
+      <c r="A37" s="8">
         <v>32</v>
       </c>
       <c r="B37" s="3">
@@ -1931,7 +1934,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
+      <c r="A38" s="8">
         <v>33</v>
       </c>
       <c r="B38" s="3">
@@ -1948,7 +1951,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+      <c r="A39" s="8">
         <v>34</v>
       </c>
       <c r="B39" s="3">
@@ -1965,7 +1968,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
+      <c r="A40" s="8">
         <v>35</v>
       </c>
       <c r="B40" s="3">
@@ -1982,7 +1985,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
+      <c r="A41" s="8">
         <v>36</v>
       </c>
       <c r="B41" s="3">
@@ -1999,7 +2002,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+      <c r="A42" s="8">
         <v>37</v>
       </c>
       <c r="B42" s="3">
@@ -2016,7 +2019,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+      <c r="A43" s="8">
         <v>38</v>
       </c>
       <c r="B43" s="3">
@@ -2033,7 +2036,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+      <c r="A44" s="8">
         <v>39</v>
       </c>
       <c r="B44" s="3">
@@ -2050,7 +2053,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
+      <c r="A45" s="8">
         <v>40</v>
       </c>
       <c r="B45" s="3">
@@ -2067,7 +2070,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="17">
+      <c r="A46" s="8">
         <v>41</v>
       </c>
       <c r="B46" s="3">
@@ -2084,7 +2087,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="17">
+      <c r="A47" s="8">
         <v>42</v>
       </c>
       <c r="B47" s="3">
@@ -2101,7 +2104,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
+      <c r="A48" s="8">
         <v>43</v>
       </c>
       <c r="B48" s="3">
@@ -2118,7 +2121,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
+      <c r="A49" s="8">
         <v>44</v>
       </c>
       <c r="B49" s="3">
@@ -2135,7 +2138,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
+      <c r="A50" s="8">
         <v>45</v>
       </c>
       <c r="B50" s="3">
@@ -2152,7 +2155,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
+      <c r="A51" s="8">
         <v>46</v>
       </c>
       <c r="B51" s="3">
@@ -2169,7 +2172,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+      <c r="A52" s="8">
         <v>47</v>
       </c>
       <c r="B52" s="3">
@@ -2186,7 +2189,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
+      <c r="A53" s="8">
         <v>48</v>
       </c>
       <c r="B53" s="3">
@@ -2203,7 +2206,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
+      <c r="A54" s="8">
         <v>49</v>
       </c>
       <c r="B54" s="3">
@@ -2220,7 +2223,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+      <c r="A55" s="8">
         <v>50</v>
       </c>
       <c r="B55" s="3">
@@ -2237,7 +2240,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+      <c r="A56" s="8">
         <v>51</v>
       </c>
       <c r="B56" s="3">
@@ -2254,7 +2257,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+      <c r="A57" s="8">
         <v>52</v>
       </c>
       <c r="B57" s="3">
@@ -2271,7 +2274,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="17">
+      <c r="A58" s="8">
         <v>53</v>
       </c>
       <c r="B58" s="3">
@@ -2288,7 +2291,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
+      <c r="A59" s="8">
         <v>54</v>
       </c>
       <c r="B59" s="3">
@@ -2305,7 +2308,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
+      <c r="A60" s="8">
         <v>55</v>
       </c>
       <c r="B60" s="3">
@@ -2322,7 +2325,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
+      <c r="A61" s="8">
         <v>56</v>
       </c>
       <c r="B61" s="3">
@@ -2339,7 +2342,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="17">
+      <c r="A62" s="8">
         <v>57</v>
       </c>
       <c r="B62" s="3">
@@ -2356,7 +2359,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
+      <c r="A63" s="8">
         <v>58</v>
       </c>
       <c r="B63" s="3">
@@ -2373,7 +2376,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="17">
+      <c r="A64" s="8">
         <v>59</v>
       </c>
       <c r="B64" s="3">
@@ -2390,7 +2393,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
+      <c r="A65" s="8">
         <v>60</v>
       </c>
       <c r="B65" s="3">
@@ -2407,7 +2410,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
+      <c r="A66" s="8">
         <v>61</v>
       </c>
       <c r="B66" s="3">
@@ -2424,7 +2427,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
+      <c r="A67" s="8">
         <v>62</v>
       </c>
       <c r="B67" s="3">
@@ -2441,7 +2444,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
+      <c r="A68" s="8">
         <v>63</v>
       </c>
       <c r="B68" s="3">
@@ -2458,7 +2461,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
+      <c r="A69" s="8">
         <v>64</v>
       </c>
       <c r="B69" s="3">
@@ -2475,7 +2478,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
+      <c r="A70" s="8">
         <v>65</v>
       </c>
       <c r="B70" s="3">
@@ -2492,7 +2495,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
+      <c r="A71" s="8">
         <v>66</v>
       </c>
       <c r="B71" s="3">
@@ -2509,7 +2512,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="17">
+      <c r="A72" s="8">
         <v>67</v>
       </c>
       <c r="B72" s="3">
@@ -2526,7 +2529,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="17">
+      <c r="A73" s="8">
         <v>68</v>
       </c>
       <c r="B73" s="3">
@@ -2543,7 +2546,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="17">
+      <c r="A74" s="8">
         <v>69</v>
       </c>
       <c r="B74" s="3">
@@ -2560,7 +2563,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
+      <c r="A75" s="8">
         <v>70</v>
       </c>
       <c r="B75" s="3">
@@ -2577,7 +2580,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="17">
+      <c r="A76" s="8">
         <v>71</v>
       </c>
       <c r="B76" s="3">
@@ -2594,7 +2597,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="18">
+      <c r="A77" s="13">
         <v>72</v>
       </c>
       <c r="B77" s="5">
@@ -2640,610 +2643,610 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="18">
         <v>43453</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="8">
         <v>0</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>1</v>
-      </c>
-      <c r="B5" s="25">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="8">
         <v>4</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="8">
         <v>5</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="8">
         <v>6</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="8">
         <v>7</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="8">
         <v>8</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+      <c r="A13" s="8">
         <v>9</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+      <c r="A14" s="8">
         <v>10</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="A15" s="8">
         <v>11</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+      <c r="A16" s="8">
         <v>12</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+      <c r="A17" s="8">
         <v>13</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="A18" s="8">
         <v>14</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+      <c r="A19" s="8">
         <v>15</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+      <c r="A20" s="8">
         <v>16</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="A21" s="8">
         <v>17</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+      <c r="A22" s="8">
         <v>18</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+      <c r="A23" s="8">
         <v>19</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+      <c r="A24" s="8">
         <v>20</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
+      <c r="A25" s="8">
         <v>21</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+      <c r="A26" s="8">
         <v>22</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+      <c r="A27" s="8">
         <v>23</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
+      <c r="A28" s="8">
         <v>24</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
+      <c r="A29" s="8">
         <v>25</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+      <c r="A30" s="8">
         <v>26</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
+      <c r="A31" s="8">
         <v>27</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+      <c r="A32" s="8">
         <v>28</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
+      <c r="A33" s="8">
         <v>29</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
+      <c r="A34" s="8">
         <v>30</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
+      <c r="A35" s="8">
         <v>31</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+      <c r="A36" s="8">
         <v>32</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
+      <c r="A37" s="8">
         <v>33</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B37" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
+      <c r="A38" s="8">
         <v>34</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B38" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+      <c r="A39" s="8">
         <v>35</v>
       </c>
-      <c r="B39" s="25">
+      <c r="B39" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
+      <c r="A40" s="8">
         <v>36</v>
       </c>
-      <c r="B40" s="25">
+      <c r="B40" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
+      <c r="A41" s="8">
         <v>37</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+      <c r="A42" s="8">
         <v>38</v>
       </c>
-      <c r="B42" s="25">
+      <c r="B42" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+      <c r="A43" s="8">
         <v>39</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+      <c r="A44" s="8">
         <v>40</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
+      <c r="A45" s="8">
         <v>41</v>
       </c>
-      <c r="B45" s="25">
+      <c r="B45" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="17">
+      <c r="A46" s="8">
         <v>42</v>
       </c>
-      <c r="B46" s="25">
+      <c r="B46" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="17">
+      <c r="A47" s="8">
         <v>43</v>
       </c>
-      <c r="B47" s="25">
+      <c r="B47" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
+      <c r="A48" s="8">
         <v>44</v>
       </c>
-      <c r="B48" s="25">
+      <c r="B48" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
+      <c r="A49" s="8">
         <v>45</v>
       </c>
-      <c r="B49" s="25">
+      <c r="B49" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
+      <c r="A50" s="8">
         <v>46</v>
       </c>
-      <c r="B50" s="25">
+      <c r="B50" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
+      <c r="A51" s="8">
         <v>47</v>
       </c>
-      <c r="B51" s="25">
+      <c r="B51" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+      <c r="A52" s="8">
         <v>48</v>
       </c>
-      <c r="B52" s="25">
+      <c r="B52" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
+      <c r="A53" s="8">
         <v>49</v>
       </c>
-      <c r="B53" s="25">
+      <c r="B53" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
+      <c r="A54" s="8">
         <v>50</v>
       </c>
-      <c r="B54" s="25">
+      <c r="B54" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+      <c r="A55" s="8">
         <v>51</v>
       </c>
-      <c r="B55" s="25">
+      <c r="B55" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+      <c r="A56" s="8">
         <v>52</v>
       </c>
-      <c r="B56" s="25">
+      <c r="B56" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+      <c r="A57" s="8">
         <v>53</v>
       </c>
-      <c r="B57" s="25">
+      <c r="B57" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="17">
+      <c r="A58" s="8">
         <v>54</v>
       </c>
-      <c r="B58" s="25">
+      <c r="B58" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
+      <c r="A59" s="8">
         <v>55</v>
       </c>
-      <c r="B59" s="25">
+      <c r="B59" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
+      <c r="A60" s="8">
         <v>56</v>
       </c>
-      <c r="B60" s="25">
+      <c r="B60" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
+      <c r="A61" s="8">
         <v>57</v>
       </c>
-      <c r="B61" s="25">
+      <c r="B61" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="17">
+      <c r="A62" s="8">
         <v>58</v>
       </c>
-      <c r="B62" s="25">
+      <c r="B62" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
+      <c r="A63" s="8">
         <v>59</v>
       </c>
-      <c r="B63" s="25">
+      <c r="B63" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="17">
+      <c r="A64" s="8">
         <v>60</v>
       </c>
-      <c r="B64" s="25">
+      <c r="B64" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
+      <c r="A65" s="8">
         <v>61</v>
       </c>
-      <c r="B65" s="25">
+      <c r="B65" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
+      <c r="A66" s="8">
         <v>62</v>
       </c>
-      <c r="B66" s="25">
+      <c r="B66" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
+      <c r="A67" s="8">
         <v>63</v>
       </c>
-      <c r="B67" s="25">
+      <c r="B67" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
+      <c r="A68" s="8">
         <v>64</v>
       </c>
-      <c r="B68" s="25">
+      <c r="B68" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
+      <c r="A69" s="8">
         <v>65</v>
       </c>
-      <c r="B69" s="25">
+      <c r="B69" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
+      <c r="A70" s="8">
         <v>66</v>
       </c>
-      <c r="B70" s="25">
+      <c r="B70" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
+      <c r="A71" s="8">
         <v>67</v>
       </c>
-      <c r="B71" s="25">
+      <c r="B71" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="17">
+      <c r="A72" s="8">
         <v>68</v>
       </c>
-      <c r="B72" s="25">
+      <c r="B72" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="17">
+      <c r="A73" s="8">
         <v>69</v>
       </c>
-      <c r="B73" s="25">
+      <c r="B73" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="17">
+      <c r="A74" s="8">
         <v>70</v>
       </c>
-      <c r="B74" s="25">
+      <c r="B74" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
+      <c r="A75" s="8">
         <v>71</v>
       </c>
-      <c r="B75" s="25">
+      <c r="B75" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="18">
+      <c r="A76" s="13">
         <v>72</v>
       </c>
-      <c r="B76" s="25">
+      <c r="B76" s="20">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3279,114 +3282,114 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="19" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="19" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EDSF-53: Swapped out images for SVGs and added animation kits for other browser
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-Scenario-Data.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-Scenario-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51C01B8-E0FD-41F8-BDB6-8CED515BEC87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C41FC-D453-400B-BA2C-1049ABAEA3C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2730" windowWidth="14670" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="2" r:id="rId1"/>
@@ -774,12 +774,12 @@
   </sheetPr>
   <dimension ref="B2:Y9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C8" sqref="C8"/>
       <selection pane="topRight" activeCell="C8" sqref="C8"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,8 +1158,8 @@
   </sheetPr>
   <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1190,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="3">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D3" s="8">
         <v>12</v>

</xml_diff>